<commit_message>
Adição do resumo da votação
Um resumo é apresentado.
</commit_message>
<xml_diff>
--- a/Relatorio_eleicao_atletica2023.xlsx
+++ b/Relatorio_eleicao_atletica2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2022004547</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -479,12 +479,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2023001138</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -512,12 +512,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2019018872</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -545,12 +545,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2023000239</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -578,12 +578,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2022004420</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -611,12 +611,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2023010450</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -644,12 +644,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>2023004087</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -677,12 +677,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>SISTEMAS DE INFORMAÇÃO/CAMP/CAMB</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A Matricula é diferente da informada.</t>
+          <t>Voto Valido.</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Arquivo Não Encontrado.</t>
+          <t>Arquivo Invalido</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -726,6 +726,74 @@
       <c r="G9" t="inlineStr">
         <is>
           <t>A Matricula é diferente da informada.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Total de Votos Validos</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Votos por Chapa</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{'Nova Era': 6, 'Branco': 1}</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Nova Era</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Chapa Vencedora</t>
         </is>
       </c>
     </row>

</xml_diff>